<commit_message>
US 3.3 commit files
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8565" yWindow="0" windowWidth="17040" windowHeight="13875"/>
+    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="4" r:id="rId2"/>
-    <sheet name="VoaSL" sheetId="3" r:id="rId3"/>
+    <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
@@ -29,9 +39,24 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>U.S. Environmental Protection Agency</t>
+  </si>
+  <si>
+    <t>Frequently Asked Questions on Mortality Risk Valuation</t>
+  </si>
+  <si>
+    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
+  </si>
+  <si>
+    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
+    <t>"What value of statistical life does EPA use?"</t>
+  </si>
+  <si>
     <t>Statistical Life</t>
   </si>
   <si>
@@ -50,56 +75,20 @@
     <t>Currency Year Adjustment</t>
   </si>
   <si>
-    <t xml:space="preserve">Government of Canada </t>
-  </si>
-  <si>
-    <t>Economic Valuation of Mortality Risk Reduction: Review and Recommendations for Policy and Regulatory Analysis</t>
-  </si>
-  <si>
-    <t>http://www.horizons.gc.ca/en/content/4-conclusions-and-recommendations-canadian-policy-analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low </t>
-  </si>
-  <si>
-    <t>central</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>We adjust 2007 dollars to 2015 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See cpi.xlsx in the InputData folder for source information </t>
-  </si>
-  <si>
-    <t>Value (CAD 2015$)</t>
-  </si>
-  <si>
-    <t>Estimate</t>
+    <t>2012$/life</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>CAD 2007$</t>
-  </si>
-  <si>
-    <t>For the Canada EPS, three VoaSL values are provided.  We choose to use the</t>
-  </si>
-  <si>
-    <t>middle estimate.</t>
+    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,27 +112,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -162,18 +130,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,18 +145,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -204,6 +155,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -252,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +239,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -495,12 +483,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
   </cols>
@@ -515,201 +503,121 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2017</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>10</v>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>4</v>
+      <c r="A9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>23</v>
+      <c r="A15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
+      <c r="A17">
+        <v>1.141</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>1.135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" location="whatvalue" display="https://www.epa.gov/environmental-economics/mortality-risk-valuation - whatvalue" xr:uid="{F4EA8DF9-36E3-4A47-8B4C-6E99399B200A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3500000</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2">
-        <v>6500000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2">
-        <v>9500000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <f>Data!B3*About!A19</f>
-        <v>7377500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+        <f>7.4*10^6*About!A17</f>
+        <v>8443400</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
custom canada files through 5/31
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\VoaSL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59E064-EF61-4312-82D8-C31F8060157D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_8218DF7238D376A0FE7EC984D2814F361A07EC1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38C523B7-6D13-4E86-BEB6-C34EE1608CD2}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="975" windowWidth="25830" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8565" yWindow="0" windowWidth="17040" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="4" r:id="rId2"/>
+    <sheet name="VoaSL" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,14 +20,19 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
@@ -39,56 +40,80 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>U.S. Environmental Protection Agency</t>
-  </si>
-  <si>
-    <t>Frequently Asked Questions on Mortality Risk Valuation</t>
-  </si>
-  <si>
-    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+    <t xml:space="preserve">Government of Canada </t>
+  </si>
+  <si>
+    <t>Economic Valuation of Mortality Risk Reduction: Review and Recommendations for Policy and Regulatory Analysis</t>
+  </si>
+  <si>
+    <t>http://www.horizons.gc.ca/en/content/4-conclusions-and-recommendations-canadian-policy-analysis</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>"What value of statistical life does EPA use?"</t>
+    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
+  </si>
+  <si>
+    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
+  </si>
+  <si>
+    <t>here must reflect the one used to calculate the health impacts in that</t>
+  </si>
+  <si>
+    <t>variable for the result to be accurate.</t>
+  </si>
+  <si>
+    <t>For the Canada EPS, three VoaSL values are provided.  We choose to use the</t>
+  </si>
+  <si>
+    <t>middle estimate.</t>
+  </si>
+  <si>
+    <t>see cpi file for currency conversions</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Conversion to 2012 USD</t>
+  </si>
+  <si>
+    <t>Conversion factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low </t>
+  </si>
+  <si>
+    <t>CAD 2007$</t>
+  </si>
+  <si>
+    <t>central</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>2012$/life</t>
   </si>
   <si>
     <t>Statistical Life</t>
   </si>
   <si>
-    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
-  </si>
-  <si>
-    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
-  </si>
-  <si>
-    <t>here must reflect the one used to calculate the health impacts in that</t>
-  </si>
-  <si>
-    <t>variable for the result to be accurate.</t>
-  </si>
-  <si>
-    <t>Currency Year Adjustment</t>
-  </si>
-  <si>
-    <t>2012$/life</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>https://www.epa.gov/environmental-economics/mortality-risk-valuation#whatvalue</t>
+    <t>Value (CAD 2015$)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +137,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,11 +182,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -144,9 +203,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -484,21 +552,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -506,118 +576,497 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="B4" s="2">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
+    <row r="20" spans="1:1">
+      <c r="A20" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" location="whatvalue" display="https://www.epa.gov/environmental-economics/mortality-risk-valuation - whatvalue" xr:uid="{F4EA8DF9-36E3-4A47-8B4C-6E99399B200A}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3500000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <f>B2*$E$2</f>
+        <v>3622644.9525000001</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1.035041415</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6500000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D4" si="0">B3*$E$2</f>
+        <v>6727769.1974999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9500000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>9832893.4425000008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <f>7.4*10^6*About!A17</f>
-        <v>8443400</v>
-      </c>
+        <f>Data!D3</f>
+        <v>6727769.1974999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6681120aa8fa62dd7a0beb503524cb55">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b98e8ac0331400a99b3dbea3ee620024" ns2:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
+    <xsd:import namespace="de340059-046a-4f1a-8b62-ade039df3700"/>
+    <xsd:import namespace="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:l787e5950a9249679d0130235a9a791b" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:ff7c4ad8664a4671b57370e258acad6a" minOccurs="0"/>
+                <xsd:element ref="ns2:of2ed5e60f3c4f8984f283882cb94320" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="52604411-7aeb-406e-8b34-4ce79a7293cc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="l787e5950a9249679d0130235a9a791b" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="l787e5950a9249679d0130235a9a791b" ma:taxonomyFieldName="ProposedRetention" ma:displayName="ProposedRetention" ma:default="" ma:fieldId="{5787e595-0a92-4967-9d01-30235a9a791b}" ma:sspId="a296b89e-8abc-49db-b68e-edd9bb7809e5" ma:termSetId="1899fd67-b032-445b-9d35-9f66b9475fa9" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e351e87d-f0a7-48fd-ab84-339d8843ff25}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="d580559a-617d-4d7d-8fb9-71ff64b58360">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="ff7c4ad8664a4671b57370e258acad6a" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="ff7c4ad8664a4671b57370e258acad6a" ma:taxonomyFieldName="Region" ma:displayName="Region" ma:default="" ma:fieldId="{ff7c4ad8-664a-4671-b573-70e258acad6a}" ma:sspId="a296b89e-8abc-49db-b68e-edd9bb7809e5" ma:termSetId="d0ef5e64-ccf8-4d0f-8f9e-d1bc0965d8f9" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="of2ed5e60f3c4f8984f283882cb94320" ma:index="14" nillable="true" ma:taxonomy="true" ma:internalName="of2ed5e60f3c4f8984f283882cb94320" ma:taxonomyFieldName="Topics" ma:displayName="Topics" ma:default="" ma:fieldId="{8f2ed5e6-0f3c-4f89-84f2-83882cb94320}" ma:taxonomyMulti="true" ma:sspId="a296b89e-8abc-49db-b68e-edd9bb7809e5" ma:termSetId="638057b0-b21b-42a9-a985-95f1f9da3292" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="de340059-046a-4f1a-8b62-ade039df3700" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="15" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="16" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="21" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="22" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="23" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d580559a-617d-4d7d-8fb9-71ff64b58360" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AEFA868-5EAE-4649-A8C1-B96AEC308AD8}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31A94240-BF0E-48AD-8DF3-E20E094CD57C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AC6A89D-8677-4BD8-A669-0AAE01875A47}"/>
 </file>
</xml_diff>